<commit_message>
Code Lists v8.2 doing
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF40D89-93A4-4705-BFD6-C257AE17FF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ABD618-C87E-4448-AD57-EBB94390F22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="519">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1583,12 +1583,57 @@
   <si>
     <t>Logistics Weight Statement</t>
   </si>
+  <si>
+    <t>PL Dokument pomocniczy ver. 1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:UtilityStatement-2::UtilityStatement##urn:fdc:www.efaktura.gov.pl:ver2.0:trns:us:ver1.0::2.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver2.0:us:ver1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderChange-2::OrderChange##urn:fdc:peppol.eu:poacc:trns:order_change:3::2.3</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderCancellation-2::OrderCancellation##urn:fdc:peppol.eu:poacc:trns:order_cancellation:3::2.3</t>
+  </si>
+  <si>
+    <t>Order Change</t>
+  </si>
+  <si>
+    <t>Order Cancellation</t>
+  </si>
+  <si>
+    <t>Order Response Advanced</t>
+  </si>
+  <si>
+    <t>TICC-219</t>
+  </si>
+  <si>
+    <t>TICC-216</t>
+  </si>
+  <si>
+    <t>Order Advanced</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:fdc:peppol.eu:poacc:trns:order:3::2.3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:advanced_ordering:3</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderResponse-2::OrderResponse##urn:fdc:peppol.eu:poacc:trns:order_response_advanced:3::2.3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1644,6 +1689,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1671,10 +1723,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1747,10 +1800,11 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Standard 3" xfId="2" xr:uid="{8757061E-72AB-4191-9614-3313A86B1B18}"/>
+    <cellStyle name="Standard 4" xfId="3" xr:uid="{D65691AB-2DBB-4DDB-972E-9107E6244D71}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2155,11 +2209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L184"/>
+  <dimension ref="A1:L189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A182" sqref="A182:A184"/>
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7817,6 +7871,163 @@
         <v>499</v>
       </c>
     </row>
+    <row r="185" spans="1:12" ht="30">
+      <c r="A185" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D185" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="H185" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="I185" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K185" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L185" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" ht="30">
+      <c r="A186" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C186" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="D186" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="E186" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="H186" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="I186" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J186" s="5">
+        <v>3</v>
+      </c>
+      <c r="K186" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L186" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" ht="30">
+      <c r="A187" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C187" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="D187" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="E187" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="H187" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="I187" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J187" s="5">
+        <v>3</v>
+      </c>
+      <c r="K187" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L187" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" ht="30">
+      <c r="A188" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="D188" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="E188" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="H188" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="I188" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J188" s="5">
+        <v>3</v>
+      </c>
+      <c r="K188" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L188" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12">
+      <c r="A189" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="D189" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="E189" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="H189" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="I189" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J189" s="5">
+        <v>3</v>
+      </c>
+      <c r="K189" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L189" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L173" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed Advanced Order; added SETU Invoice v2.2; TICC-217
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E70D93-98C7-47FC-826F-E34879F4A8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52137160-43C6-403C-9B7C-067549A7152D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="512">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1505,123 +1505,107 @@
     <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver2.0:us:ver1.0</t>
   </si>
   <si>
-    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderChange-2::OrderChange##urn:fdc:peppol.eu:poacc:trns:order_change:3::2.3</t>
-  </si>
-  <si>
-    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderCancellation-2::OrderCancellation##urn:fdc:peppol.eu:poacc:trns:order_cancellation:3::2.3</t>
-  </si>
-  <si>
-    <t>TICC-219</t>
-  </si>
-  <si>
     <t>TICC-216</t>
   </si>
   <si>
-    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:advanced_ordering:3</t>
-  </si>
-  <si>
-    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderResponse-2::OrderResponse##urn:fdc:peppol.eu:poacc:trns:order_response_advanced:3::2.3</t>
+    <t>Peppol Invoice Response V1</t>
+  </si>
+  <si>
+    <t>Peppol Catalogue transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Catalogue Response transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Order transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Invoice Response transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Order Response transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Punch Out transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Despatch Advice transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Order Agreement transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol Message Level Response transaction 3.0</t>
+  </si>
+  <si>
+    <t>Peppol BIS Billing UBL Invoice V3</t>
+  </si>
+  <si>
+    <t>Peppol BIS Billing UBL CreditNote V3</t>
+  </si>
+  <si>
+    <t>Peppol BIS Billing CII Invoice V3</t>
+  </si>
+  <si>
+    <t>SG Peppol BIS Billing 3.0 Invoice</t>
+  </si>
+  <si>
+    <t>SG Peppol BIS Billing 3.0 Credit Note</t>
+  </si>
+  <si>
+    <t>AU-NZ Peppol BIS Billing 3.0 Invoice</t>
+  </si>
+  <si>
+    <t>AU-NZ Peppol BIS Billing 3.0 CreditNote</t>
+  </si>
+  <si>
+    <t>Peppol Tendering Questions V1.0</t>
+  </si>
+  <si>
+    <t>Peppol Tendering Answers V1.0</t>
+  </si>
+  <si>
+    <t>Peppol Tender Clarification Request V1.0</t>
+  </si>
+  <si>
+    <t>Peppol Tender Clarification Response V1.0</t>
+  </si>
+  <si>
+    <t>Peppol End User Report</t>
+  </si>
+  <si>
+    <t>Peppol Transaction Statistics Report</t>
+  </si>
+  <si>
+    <t>Peppol Tender Submission Tender V1</t>
+  </si>
+  <si>
+    <t>Peppol Tender Submission TenderReceipt V1</t>
+  </si>
+  <si>
+    <t>Peppol Procurement document access CallForTenders V1</t>
+  </si>
+  <si>
+    <t>Peppol Procurement document access TenderStatusRequest V1</t>
+  </si>
+  <si>
+    <t>Peppol Procurement procedure subscription Response V1</t>
+  </si>
+  <si>
+    <t>Peppol Procurement procedure subscription Request V1</t>
   </si>
   <si>
     <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:ordering:3
-cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_only:3
-cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:advanced_ordering:3</t>
-  </si>
-  <si>
-    <t>Peppol Invoice Response V1</t>
-  </si>
-  <si>
-    <t>Peppol Catalogue transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Catalogue Response transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Order transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Invoice Response transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Order Response transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Punch Out transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Despatch Advice transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Order Agreement transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol Message Level Response transaction 3.0</t>
-  </si>
-  <si>
-    <t>Peppol BIS Billing UBL Invoice V3</t>
-  </si>
-  <si>
-    <t>Peppol BIS Billing UBL CreditNote V3</t>
-  </si>
-  <si>
-    <t>Peppol BIS Billing CII Invoice V3</t>
-  </si>
-  <si>
-    <t>SG Peppol BIS Billing 3.0 Invoice</t>
-  </si>
-  <si>
-    <t>SG Peppol BIS Billing 3.0 Credit Note</t>
-  </si>
-  <si>
-    <t>AU-NZ Peppol BIS Billing 3.0 Invoice</t>
-  </si>
-  <si>
-    <t>AU-NZ Peppol BIS Billing 3.0 CreditNote</t>
-  </si>
-  <si>
-    <t>Peppol Order Change</t>
-  </si>
-  <si>
-    <t>Peppol Order Cancellation</t>
-  </si>
-  <si>
-    <t>Peppol Order Response Advanced</t>
-  </si>
-  <si>
-    <t>Peppol Tendering Questions V1.0</t>
-  </si>
-  <si>
-    <t>Peppol Tendering Answers V1.0</t>
-  </si>
-  <si>
-    <t>Peppol Tender Clarification Request V1.0</t>
-  </si>
-  <si>
-    <t>Peppol Tender Clarification Response V1.0</t>
-  </si>
-  <si>
-    <t>Peppol End User Report</t>
-  </si>
-  <si>
-    <t>Peppol Transaction Statistics Report</t>
-  </si>
-  <si>
-    <t>Peppol Tender Submission Tender V1</t>
-  </si>
-  <si>
-    <t>Peppol Tender Submission TenderReceipt V1</t>
-  </si>
-  <si>
-    <t>Peppol Procurement document access CallForTenders V1</t>
-  </si>
-  <si>
-    <t>Peppol Procurement document access TenderStatusRequest V1</t>
-  </si>
-  <si>
-    <t>Peppol Procurement procedure subscription Response V1</t>
-  </si>
-  <si>
-    <t>Peppol Procurement procedure subscription Request V1</t>
+cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_only:3</t>
+  </si>
+  <si>
+    <t>SETU Invoice v2.2</t>
+  </si>
+  <si>
+    <t>TICC-217</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:nen.nl:nlcius:v1.0#compliant#urn:fdc:setu.nl:invoice:v2.2::2.1</t>
   </si>
 </sst>
 </file>
@@ -2207,7 +2191,7 @@
   <dimension ref="A1:L188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A186" sqref="A186"/>
     </sheetView>
   </sheetViews>
@@ -3255,7 +3239,7 @@
     </row>
     <row r="32" spans="1:12" ht="30">
       <c r="A32" s="5" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>56</v>
@@ -3285,7 +3269,7 @@
     </row>
     <row r="33" spans="1:12" ht="30">
       <c r="A33" s="5" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>56</v>
@@ -3405,7 +3389,7 @@
     </row>
     <row r="37" spans="1:12" ht="30">
       <c r="A37" s="5" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>56</v>
@@ -3435,7 +3419,7 @@
     </row>
     <row r="38" spans="1:12" ht="45">
       <c r="A38" s="5" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>56</v>
@@ -3465,7 +3449,7 @@
     </row>
     <row r="39" spans="1:12" ht="45">
       <c r="A39" s="5" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>56</v>
@@ -3495,7 +3479,7 @@
     </row>
     <row r="40" spans="1:12" ht="45">
       <c r="A40" s="5" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>56</v>
@@ -3525,7 +3509,7 @@
     </row>
     <row r="41" spans="1:12" ht="45">
       <c r="A41" s="5" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>56</v>
@@ -3555,7 +3539,7 @@
     </row>
     <row r="42" spans="1:12" ht="45">
       <c r="A42" s="5" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>56</v>
@@ -3585,7 +3569,7 @@
     </row>
     <row r="43" spans="1:12" ht="45">
       <c r="A43" s="5" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>56</v>
@@ -3834,7 +3818,7 @@
     </row>
     <row r="51" spans="1:12" ht="30">
       <c r="A51" s="5" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>56</v>
@@ -3867,7 +3851,7 @@
     </row>
     <row r="52" spans="1:12" ht="30">
       <c r="A52" s="5" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>56</v>
@@ -3897,7 +3881,7 @@
     </row>
     <row r="53" spans="1:12" ht="30">
       <c r="A53" s="5" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>56</v>
@@ -3925,9 +3909,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="45">
+    <row r="54" spans="1:12" ht="30">
       <c r="A54" s="5" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>56</v>
@@ -3941,9 +3925,6 @@
       <c r="E54" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>480</v>
-      </c>
       <c r="I54" s="5" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3955,12 +3936,12 @@
         <v>117</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>484</v>
+        <v>508</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="30">
       <c r="A55" s="5" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>56</v>
@@ -3990,7 +3971,7 @@
     </row>
     <row r="56" spans="1:12" ht="30">
       <c r="A56" s="5" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>56</v>
@@ -4020,7 +4001,7 @@
     </row>
     <row r="57" spans="1:12" ht="30">
       <c r="A57" s="5" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>56</v>
@@ -4050,7 +4031,7 @@
     </row>
     <row r="58" spans="1:12" ht="30">
       <c r="A58" s="5" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>56</v>
@@ -4080,7 +4061,7 @@
     </row>
     <row r="59" spans="1:12" ht="30">
       <c r="A59" s="5" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>56</v>
@@ -4110,7 +4091,7 @@
     </row>
     <row r="60" spans="1:12" ht="30">
       <c r="A60" s="5" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>56</v>
@@ -4194,7 +4175,7 @@
     </row>
     <row r="63" spans="1:12" ht="30">
       <c r="A63" s="5" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>56</v>
@@ -4260,7 +4241,7 @@
     </row>
     <row r="65" spans="1:12" ht="45">
       <c r="A65" s="5" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>56</v>
@@ -4473,7 +4454,7 @@
     </row>
     <row r="72" spans="1:12" ht="45">
       <c r="A72" s="8" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>56</v>
@@ -4506,7 +4487,7 @@
     </row>
     <row r="73" spans="1:12" ht="45">
       <c r="A73" s="8" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>56</v>
@@ -6264,7 +6245,7 @@
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="15" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>56</v>
@@ -6296,7 +6277,7 @@
     </row>
     <row r="131" spans="1:12" ht="30">
       <c r="A131" s="15" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>56</v>
@@ -6328,7 +6309,7 @@
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="15" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>56</v>
@@ -6360,7 +6341,7 @@
     </row>
     <row r="133" spans="1:12" ht="30">
       <c r="A133" s="15" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>56</v>
@@ -7726,7 +7707,7 @@
     </row>
     <row r="180" spans="1:12">
       <c r="A180" s="5" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="B180" s="4" t="s">
         <v>56</v>
@@ -7755,7 +7736,7 @@
     </row>
     <row r="181" spans="1:12" ht="30">
       <c r="A181" s="5" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="B181" s="4" t="s">
         <v>56</v>
@@ -7886,7 +7867,7 @@
         <v>374</v>
       </c>
       <c r="H185" s="5" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="I185" s="5" t="b">
         <v>0</v>
@@ -7898,15 +7879,15 @@
         <v>477</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="30">
+    <row r="186" spans="1:12" ht="45">
       <c r="A186" s="5" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="B186" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>478</v>
+        <v>511</v>
       </c>
       <c r="D186" s="21" t="s">
         <v>476</v>
@@ -7915,84 +7896,23 @@
         <v>374</v>
       </c>
       <c r="H186" s="5" t="s">
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="I186" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J186" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K186" s="5" t="s">
         <v>117</v>
       </c>
       <c r="L186" s="5" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="187" spans="1:12" ht="30">
-      <c r="A187" s="5" t="s">
-        <v>503</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C187" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="D187" s="21" t="s">
-        <v>476</v>
-      </c>
-      <c r="E187" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="H187" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="I187" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J187" s="5">
-        <v>3</v>
-      </c>
-      <c r="K187" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L187" s="5" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="188" spans="1:12" ht="30">
-      <c r="A188" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C188" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="D188" s="21" t="s">
-        <v>476</v>
-      </c>
-      <c r="E188" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="H188" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="I188" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J188" s="5">
-        <v>3</v>
-      </c>
-      <c r="K188" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L188" s="5" t="s">
-        <v>482</v>
-      </c>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12">
+      <c r="B187" s="4"/>
+    </row>
+    <row r="188" spans="1:12">
+      <c r="B188" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L188" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Added JP PINT Invoice; TICC-222
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52137160-43C6-403C-9B7C-067549A7152D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C5D990-6F17-43AD-9EAE-3E611BB6F667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="515">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1606,6 +1606,15 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:nen.nl:nlcius:v1.0#compliant#urn:fdc:setu.nl:invoice:v2.2::2.1</t>
+  </si>
+  <si>
+    <t>JP PINT invoice</t>
+  </si>
+  <si>
+    <t>TICC-222</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:fdc:peppol:jp:billing:3.0::2.1</t>
   </si>
 </sst>
 </file>
@@ -2191,8 +2200,8 @@
   <dimension ref="A1:L188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A186" sqref="A186"/>
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7909,7 +7918,37 @@
       </c>
     </row>
     <row r="187" spans="1:12">
-      <c r="B187" s="4"/>
+      <c r="A187" t="s">
+        <v>512</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C187" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="D187" s="21" t="s">
+        <v>476</v>
+      </c>
+      <c r="E187" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="H187" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="I187" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="J187" s="5">
+        <v>3</v>
+      </c>
+      <c r="K187" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L187" s="7" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="188" spans="1:12">
       <c r="B188" s="4"/>

</xml_diff>

<commit_message>
Ensured row is empty
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C5D990-6F17-43AD-9EAE-3E611BB6F667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E332F360-767C-45BF-9F07-B0BB059D0EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$188</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$187</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -2197,11 +2197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L188"/>
+  <dimension ref="A1:L187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A188" sqref="A188"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7950,11 +7950,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="188" spans="1:12">
-      <c r="B188" s="4"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L188" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L187" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>